<commit_message>
chore: Fix blueprint parameter sorting
</commit_message>
<xml_diff>
--- a/ArqVJ2026/Assets/StreamingAssets/Blueprints/Blueprints.xlsx
+++ b/ArqVJ2026/Assets/StreamingAssets/Blueprints/Blueprints.xlsx
@@ -4,19 +4,20 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Animals" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="DayNightCycle" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="leEm6sv2E6LpVMA6wUmGkdBnkV3RDAZ4fuQX+ybbqFQ="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="D9Ls52x18aKXvfH+R5YCmcEqaIWPP7zib9pKadSAYkA="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>IDS</t>
   </si>
@@ -46,6 +47,33 @@
   </si>
   <si>
     <t>Piolin!</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Mañana</t>
+  </si>
+  <si>
+    <t>Manana</t>
+  </si>
+  <si>
+    <t>Mediodía</t>
+  </si>
+  <si>
+    <t>Mediodia</t>
+  </si>
+  <si>
+    <t>Tarde</t>
+  </si>
+  <si>
+    <t>Atardecer</t>
+  </si>
+  <si>
+    <t>Anochecer</t>
+  </si>
+  <si>
+    <t>Madrugada</t>
   </si>
 </sst>
 </file>
@@ -78,13 +106,25 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -95,6 +135,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1373,4 +1417,96 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="5">
+        <v>24.0</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="5">
+        <v>24.0</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="5">
+        <v>24.0</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5">
+        <v>24.0</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5">
+        <v>24.0</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="5">
+        <v>24.0</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Tiled map class implementation
</commit_message>
<xml_diff>
--- a/ArqVJ2026/Assets/StreamingAssets/Blueprints/Blueprints.xlsx
+++ b/ArqVJ2026/Assets/StreamingAssets/Blueprints/Blueprints.xlsx
@@ -5,19 +5,20 @@
   <sheets>
     <sheet state="visible" name="Animals" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="DayNightCycle" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Tile Types" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="D9Ls52x18aKXvfH+R5YCmcEqaIWPP7zib9pKadSAYkA="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="3ocmGzteBs5wA4cTWB+Jp905mPVE+wqPKieSPUyFjVU="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>IDS</t>
   </si>
@@ -74,13 +75,49 @@
   </si>
   <si>
     <t>Madrugada</t>
+  </si>
+  <si>
+    <t>Is Structure</t>
+  </si>
+  <si>
+    <t>Is Walkable</t>
+  </si>
+  <si>
+    <t>Is Animal Habitat</t>
+  </si>
+  <si>
+    <t>Can Spawn Humans</t>
+  </si>
+  <si>
+    <t>Can Dispawn Humans</t>
+  </si>
+  <si>
+    <t>Road</t>
+  </si>
+  <si>
+    <t>Jail Walls</t>
+  </si>
+  <si>
+    <t>Jail Habitat</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>Humans Entry</t>
+  </si>
+  <si>
+    <t>Humans Exit</t>
+  </si>
+  <si>
+    <t>Grass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -90,6 +127,11 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -106,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -126,6 +168,9 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -139,6 +184,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1509,4 +1558,179 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Factory event registration with Reflection
</commit_message>
<xml_diff>
--- a/ArqVJ2026/Assets/StreamingAssets/Blueprints/Blueprints.xlsx
+++ b/ArqVJ2026/Assets/StreamingAssets/Blueprints/Blueprints.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>IDS</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Can Dispawn Humans</t>
+  </si>
+  <si>
+    <t>Is Default</t>
   </si>
   <si>
     <t>Road</t>
@@ -1589,10 +1592,13 @@
       <c r="F1" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="G1" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="7" t="b">
         <v>0</v>
@@ -1609,10 +1615,13 @@
       <c r="F2" s="7" t="b">
         <v>0</v>
       </c>
+      <c r="G2" s="7" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" s="7" t="b">
         <v>1</v>
@@ -1629,10 +1638,13 @@
       <c r="F3" s="7" t="b">
         <v>0</v>
       </c>
+      <c r="G3" s="7" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" s="7" t="b">
         <v>0</v>
@@ -1649,10 +1661,13 @@
       <c r="F4" s="7" t="b">
         <v>0</v>
       </c>
+      <c r="G4" s="7" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B5" s="7" t="b">
         <v>1</v>
@@ -1669,10 +1684,13 @@
       <c r="F5" s="7" t="b">
         <v>0</v>
       </c>
+      <c r="G5" s="7" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B6" s="7" t="b">
         <v>0</v>
@@ -1689,10 +1707,13 @@
       <c r="F6" s="7" t="b">
         <v>0</v>
       </c>
+      <c r="G6" s="7" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="7" t="b">
         <v>0</v>
@@ -1709,10 +1730,13 @@
       <c r="F7" s="7" t="b">
         <v>1</v>
       </c>
+      <c r="G7" s="7" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" s="7" t="b">
         <v>0</v>
@@ -1728,6 +1752,9 @@
       </c>
       <c r="F8" s="7" t="b">
         <v>0</v>
+      </c>
+      <c r="G8" s="7" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Entity view and view classes
</commit_message>
<xml_diff>
--- a/ArqVJ2026/Assets/StreamingAssets/Blueprints/Blueprints.xlsx
+++ b/ArqVJ2026/Assets/StreamingAssets/Blueprints/Blueprints.xlsx
@@ -4,21 +4,22 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Animals" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="DayNightCycle" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Tile Types" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Prefabs View" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="DayNightCycle" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Tile Types" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="3ocmGzteBs5wA4cTWB+Jp905mPVE+wqPKieSPUyFjVU="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="24OAQv7MQbZsF86thvXqb/dI789StRF6A52atKYYayY="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>IDS</t>
   </si>
@@ -48,6 +49,18 @@
   </si>
   <si>
     <t>Piolin!</t>
+  </si>
+  <si>
+    <t>Architecture ID</t>
+  </si>
+  <si>
+    <t>Prefab resource path</t>
+  </si>
+  <si>
+    <t>Monkey view</t>
+  </si>
+  <si>
+    <t>Entities/LivingEntities/Animals/Monkey.prefab</t>
   </si>
   <si>
     <t>Duration</t>
@@ -159,6 +172,9 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -170,9 +186,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -191,6 +204,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1485,77 +1502,22 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>3</v>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="5">
-        <v>24.0</v>
-      </c>
-      <c r="C2" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" s="5">
-        <v>24.0</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="5">
-        <v>24.0</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="5">
-        <v>24.0</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="5">
-        <v>24.0</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="5">
-        <v>24.0</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1574,186 +1536,281 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="6">
+        <v>24.0</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="6">
+        <v>24.0</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="B4" s="6">
+        <v>24.0</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="B5" s="6">
+        <v>24.0</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="B6" s="6">
+        <v>24.0</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="B7" s="6">
+        <v>24.0</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="4" max="4" width="15.13"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="C1" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="b">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="7" t="b">
+      <c r="D2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="7" t="b">
+      <c r="A3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="7" t="b">
+      <c r="C3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="7" t="b">
+      <c r="A4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E4" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="7" t="b">
+      <c r="E4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="7" t="b">
+      <c r="A5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="C5" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="7" t="b">
+      <c r="C5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" s="7" t="b">
+      <c r="A6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D6" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="7" t="b">
+      <c r="D6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="F6" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" s="7" t="b">
+      <c r="F6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" s="7" t="b">
+      <c r="A7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D7" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="7" t="b">
+      <c r="D7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="G7" s="7" t="b">
+      <c r="G7" s="3" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="7" t="b">
+      <c r="A8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D8" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" s="7" t="b">
+      <c r="D8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Spawn entity request
</commit_message>
<xml_diff>
--- a/ArqVJ2026/Assets/StreamingAssets/Blueprints/Blueprints.xlsx
+++ b/ArqVJ2026/Assets/StreamingAssets/Blueprints/Blueprints.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>IDS</t>
   </si>
@@ -61,6 +61,21 @@
   </si>
   <si>
     <t>Prefabs/Entities/LivingEntities/Animals/Monkey</t>
+  </si>
+  <si>
+    <t>Bird view</t>
+  </si>
+  <si>
+    <t>Bird</t>
+  </si>
+  <si>
+    <t>Prefabs/Entities/LivingEntities/Animals/Bird</t>
+  </si>
+  <si>
+    <t>Snake view</t>
+  </si>
+  <si>
+    <t>Prefabs/Entities/LivingEntities/Animals/Snake</t>
   </si>
   <si>
     <t>Duration</t>
@@ -1520,6 +1535,28 @@
         <v>13</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1540,7 +1577,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>3</v>
@@ -1548,68 +1585,68 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B2" s="6">
         <v>24.0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B3" s="6">
         <v>24.0</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B4" s="6">
         <v>24.0</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B5" s="6">
         <v>24.0</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B6" s="6">
         <v>24.0</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B7" s="6">
         <v>24.0</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1635,27 +1672,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="b">
         <v>0</v>
@@ -1678,7 +1715,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B3" s="3" t="b">
         <v>1</v>
@@ -1701,7 +1738,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B4" s="3" t="b">
         <v>0</v>
@@ -1724,7 +1761,7 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B5" s="3" t="b">
         <v>1</v>
@@ -1747,7 +1784,7 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B6" s="3" t="b">
         <v>0</v>
@@ -1770,7 +1807,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>0</v>
@@ -1793,7 +1830,7 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B8" s="3" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
chore: Fix missing prefab pipeline
</commit_message>
<xml_diff>
--- a/ArqVJ2026/Assets/StreamingAssets/Blueprints/Blueprints.xlsx
+++ b/ArqVJ2026/Assets/StreamingAssets/Blueprints/Blueprints.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>IDS</t>
   </si>
@@ -45,7 +45,7 @@
     <t>Jose</t>
   </si>
   <si>
-    <t>RecontraBird</t>
+    <t>Bird</t>
   </si>
   <si>
     <t>Piolin!</t>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Bird view</t>
-  </si>
-  <si>
-    <t>Bird</t>
   </si>
   <si>
     <t>Prefabs/Entities/LivingEntities/Animals/Bird</t>
@@ -476,7 +473,7 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1">
@@ -490,18 +487,10 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1">
-        <v>102.0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" ht="15.75" customHeight="1"/>
     <row r="7" ht="15.75" customHeight="1"/>
@@ -1540,21 +1529,21 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1577,7 +1566,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>3</v>
@@ -1585,68 +1574,68 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="6">
         <v>24.0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="6">
         <v>24.0</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="6">
         <v>24.0</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="6">
         <v>24.0</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="6">
         <v>24.0</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="6">
         <v>24.0</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1672,27 +1661,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="b">
         <v>0</v>
@@ -1715,7 +1704,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3" t="b">
         <v>1</v>
@@ -1738,7 +1727,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="3" t="b">
         <v>0</v>
@@ -1761,7 +1750,7 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="3" t="b">
         <v>1</v>
@@ -1784,7 +1773,7 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="3" t="b">
         <v>0</v>
@@ -1807,7 +1796,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>0</v>
@@ -1830,7 +1819,7 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="3" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
feat: Implement map visualization
</commit_message>
<xml_diff>
--- a/ArqVJ2026/Assets/StreamingAssets/Blueprints/Blueprints.xlsx
+++ b/ArqVJ2026/Assets/StreamingAssets/Blueprints/Blueprints.xlsx
@@ -7,19 +7,20 @@
     <sheet state="visible" name="Prefabs View" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="DayNightCycle" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="Tile Types" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Tiles View" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="24OAQv7MQbZsF86thvXqb/dI789StRF6A52atKYYayY="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="7LCvqTT6XfhXL7aoOqxK4QC6R7Qlsfk6BBHG2jGbRWo="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
   <si>
     <t>IDS</t>
   </si>
@@ -139,6 +140,54 @@
   </si>
   <si>
     <t>Grass</t>
+  </si>
+  <si>
+    <t>Road view</t>
+  </si>
+  <si>
+    <t>Prefabs/Map/YellowTile</t>
+  </si>
+  <si>
+    <t>Jail Walls view</t>
+  </si>
+  <si>
+    <t>Prefabs/Map/RedTile</t>
+  </si>
+  <si>
+    <t>Jail Habitat view</t>
+  </si>
+  <si>
+    <t>Prefabs/Map/CyanTile</t>
+  </si>
+  <si>
+    <t>Power Supply</t>
+  </si>
+  <si>
+    <t>Prefabs/Map/GreenTile</t>
+  </si>
+  <si>
+    <t>Humans Entry View</t>
+  </si>
+  <si>
+    <t>Human Entry</t>
+  </si>
+  <si>
+    <t>Prefabs/Map/BlueTile</t>
+  </si>
+  <si>
+    <t>Humans Exit View</t>
+  </si>
+  <si>
+    <t>Human Exit</t>
+  </si>
+  <si>
+    <t>Prefabs/Map/PinkTile</t>
+  </si>
+  <si>
+    <t>Grass View</t>
+  </si>
+  <si>
+    <t>Prefabs/Map/OrangeTile</t>
   </si>
 </sst>
 </file>
@@ -220,6 +269,10 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1843,4 +1896,107 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Context Menu First Implementation
</commit_message>
<xml_diff>
--- a/ArqVJ2026/Assets/StreamingAssets/Blueprints/Blueprints.xlsx
+++ b/ArqVJ2026/Assets/StreamingAssets/Blueprints/Blueprints.xlsx
@@ -7,20 +7,21 @@
     <sheet state="visible" name="Prefabs View" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="DayNightCycle" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="Tile Types" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Tiles View" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="UI View" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="Tiles View" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="7LCvqTT6XfhXL7aoOqxK4QC6R7Qlsfk6BBHG2jGbRWo="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="tCdN6oCBVutCUNbulb5YA+cdsqe0FCLbOuSJiq08rm4="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
   <si>
     <t>IDS</t>
   </si>
@@ -140,6 +141,24 @@
   </si>
   <si>
     <t>Grass</t>
+  </si>
+  <si>
+    <t>MENU_CONTAINER</t>
+  </si>
+  <si>
+    <t>ContextMenuContainer</t>
+  </si>
+  <si>
+    <t>Prefabs/UI/ContextMenuContainer</t>
+  </si>
+  <si>
+    <t>MENU_BUTTON</t>
+  </si>
+  <si>
+    <t>ButtonPrefab</t>
+  </si>
+  <si>
+    <t>Prefabs/UI/ButtonPrefab</t>
   </si>
   <si>
     <t>Road view</t>
@@ -273,6 +292,10 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1924,32 +1947,80 @@
         <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5">
@@ -1957,43 +2028,43 @@
         <v>36</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Spawn entities on grid coordinate
</commit_message>
<xml_diff>
--- a/ArqVJ2026/Assets/StreamingAssets/Blueprints/Blueprints.xlsx
+++ b/ArqVJ2026/Assets/StreamingAssets/Blueprints/Blueprints.xlsx
@@ -8,20 +8,21 @@
     <sheet state="visible" name="DayNightCycle" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="Tile Types" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="UI View" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Tiles View" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="Cameras View" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="Tiles View" sheetId="7" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="tCdN6oCBVutCUNbulb5YA+cdsqe0FCLbOuSJiq08rm4="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataChecksum="TgXy59lm6zdiO3USCmn6HTxfTJKGdyMkHALsW6wsLNE="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
   <si>
     <t>IDS</t>
   </si>
@@ -159,6 +160,15 @@
   </si>
   <si>
     <t>Prefabs/UI/ButtonPrefab</t>
+  </si>
+  <si>
+    <t>GAME_CAMERA</t>
+  </si>
+  <si>
+    <t>GameCamera</t>
+  </si>
+  <si>
+    <t>Prefabs/Camera/GameCamera</t>
   </si>
   <si>
     <t>Road view</t>
@@ -296,6 +306,10 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1995,32 +2009,69 @@
         <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5">
@@ -2028,43 +2079,43 @@
         <v>36</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Create controllers for single and multiple terrain selection
</commit_message>
<xml_diff>
--- a/ArqVJ2026/Assets/StreamingAssets/Blueprints/Blueprints.xlsx
+++ b/ArqVJ2026/Assets/StreamingAssets/Blueprints/Blueprints.xlsx
@@ -4,8 +4,8 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Animals" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Prefabs View" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="DayNightCycle" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Animals View" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Day Night Cycle" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="Tile Types" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="UI View" sheetId="5" r:id="rId8"/>
     <sheet state="visible" name="Cameras View" sheetId="6" r:id="rId9"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
   <si>
     <t>IDS</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Is Default</t>
+  </si>
+  <si>
+    <t>Is Unique</t>
   </si>
   <si>
     <t>Road</t>
@@ -1768,10 +1771,13 @@
       <c r="G1" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="b">
         <v>0</v>
@@ -1791,10 +1797,13 @@
       <c r="G2" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="H2" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B3" s="3" t="b">
         <v>1</v>
@@ -1814,10 +1823,13 @@
       <c r="G3" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="H3" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" s="3" t="b">
         <v>0</v>
@@ -1837,10 +1849,13 @@
       <c r="G4" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="H4" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B5" s="3" t="b">
         <v>1</v>
@@ -1860,10 +1875,13 @@
       <c r="G5" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="H5" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B6" s="3" t="b">
         <v>0</v>
@@ -1883,10 +1901,13 @@
       <c r="G6" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="H6" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>0</v>
@@ -1906,10 +1927,13 @@
       <c r="G7" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="H7" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B8" s="3" t="b">
         <v>0</v>
@@ -1928,6 +1952,9 @@
       </c>
       <c r="G8" s="3" t="b">
         <v>1</v>
+      </c>
+      <c r="H8" s="3" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1958,24 +1985,24 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2006,13 +2033,13 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2043,79 +2070,79 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>